<commit_message>
melhorei o diagrama de pesquisa por expressão
</commit_message>
<xml_diff>
--- a/use-cases/use-case-pesquisar-expressao.xlsx
+++ b/use-cases/use-case-pesquisar-expressao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepereira/Desktop/use cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepereira/src/univ/programs/projects/projeto-li4/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13F935F-E9A6-B243-ADAB-D2769E947E4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDE11DF-DB81-7E45-A02E-4BF96ED1FC50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16240" windowHeight="21600" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Actor input</t>
   </si>
@@ -55,24 +55,35 @@
     <t>Apresentar explicação ao utilizador</t>
   </si>
   <si>
-    <t>Registado no sistema, e logado no sistema, 
-ter escolhido e iniciado uma receita, 
-estar num determinado passo de uma receita</t>
-  </si>
-  <si>
-    <t>Pesquisar palavra/expressão</t>
-  </si>
-  <si>
-    <t>1. Indicar/selecionar expressão para explicação</t>
-  </si>
-  <si>
-    <t>2. Apresenta explicação da expressão</t>
-  </si>
-  <si>
-    <t>3. Indica término do processo</t>
-  </si>
-  <si>
-    <t>4. Termina explicação/processo</t>
+    <t>1. Indicar expressão para explicação</t>
+  </si>
+  <si>
+    <t>4. Termina processo</t>
+  </si>
+  <si>
+    <t>2. Validar expressão</t>
+  </si>
+  <si>
+    <t>3. Apresenta explicação da expressão</t>
+  </si>
+  <si>
+    <t>Registado/logado no sistema, 
+ter escolhido e iniciado uma receita</t>
+  </si>
+  <si>
+    <t>Pesquisar expressão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exceção 1
+(passo 2)
+[expressão inválida]
+</t>
+  </si>
+  <si>
+    <t>2.1. Informa que a expressão é inválida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2 Termina processo </t>
   </si>
 </sst>
 </file>
@@ -109,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -239,11 +250,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -256,12 +295,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,16 +325,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -600,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,40 +669,40 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="9"/>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="2:4" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="2:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="14"/>
+      <c r="C4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -663,35 +713,52 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="17"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="18"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="22" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>